<commit_message>
firma ve firma cihaz kayıt servisler ve getler hazır
</commit_message>
<xml_diff>
--- a/dosyalar/db yapısı.xlsx
+++ b/dosyalar/db yapısı.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="129">
   <si>
     <t>firma</t>
   </si>
@@ -93,12 +93,6 @@
     <t>enumCihazTip</t>
   </si>
   <si>
-    <t>cihaz_1</t>
-  </si>
-  <si>
-    <t>cihaz_2</t>
-  </si>
-  <si>
     <t>personel</t>
   </si>
   <si>
@@ -403,6 +397,15 @@
   </si>
   <si>
     <t>molaSaat</t>
+  </si>
+  <si>
+    <t>qr_cihazi</t>
+  </si>
+  <si>
+    <t>cihaz_model_1</t>
+  </si>
+  <si>
+    <t>cihaz_model_2</t>
   </si>
 </sst>
 </file>
@@ -734,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,9 +752,13 @@
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="22.7109375" customWidth="1"/>
-    <col min="13" max="14" width="12.140625" customWidth="1"/>
-    <col min="18" max="18" width="19.140625" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" customWidth="1"/>
+    <col min="16" max="16" width="18.5703125" customWidth="1"/>
+    <col min="18" max="18" width="25" customWidth="1"/>
     <col min="19" max="19" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -765,49 +772,49 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>19</v>
@@ -857,25 +864,25 @@
         <v>5</v>
       </c>
       <c r="N2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Q2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="T2" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -901,16 +908,16 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I3" t="s">
         <v>15</v>
       </c>
       <c r="J3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L3" t="s">
         <v>18</v>
@@ -919,25 +926,25 @@
         <v>4</v>
       </c>
       <c r="N3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="O3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Q3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="S3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="T3" t="s">
-        <v>25</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -951,43 +958,46 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K4" t="s">
         <v>4</v>
       </c>
       <c r="L4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M4" t="s">
         <v>2</v>
       </c>
       <c r="N4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="P4" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+      <c r="T4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -1007,16 +1017,16 @@
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K5" t="s">
         <v>2</v>
@@ -1025,10 +1035,10 @@
         <v>2</v>
       </c>
       <c r="M5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -1039,31 +1049,31 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
         <v>29</v>
       </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
       <c r="I6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L6" t="s">
         <v>4</v>
       </c>
       <c r="M6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1071,225 +1081,225 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
         <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" t="s">
         <v>125</v>
       </c>
-      <c r="F8" t="s">
-        <v>74</v>
-      </c>
-      <c r="J8" t="s">
-        <v>127</v>
-      </c>
       <c r="K8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="M9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="O10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="O11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="O13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="L17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J22" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J27" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
@@ -1297,10 +1307,10 @@
         <v>1010001</v>
       </c>
       <c r="J28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
yetki rol eklentisi ama yarım biraz bozuk ayrıca kontrollerlar yok
</commit_message>
<xml_diff>
--- a/dosyalar/db yapısı.xlsx
+++ b/dosyalar/db yapısı.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="132">
   <si>
     <t>firma</t>
   </si>
@@ -403,6 +403,18 @@
   </si>
   <si>
     <t>cihaz_model_2</t>
+  </si>
+  <si>
+    <t>rol</t>
+  </si>
+  <si>
+    <t>ekran</t>
+  </si>
+  <si>
+    <t>ekran_rol</t>
+  </si>
+  <si>
+    <t>rol_kisi</t>
   </si>
 </sst>
 </file>
@@ -732,106 +744,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S28"/>
+  <dimension ref="A1:X28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="22.7109375" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" customWidth="1"/>
-    <col min="15" max="15" width="18.5703125" customWidth="1"/>
-    <col min="17" max="17" width="25" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="22.7109375" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" customWidth="1"/>
+    <col min="18" max="18" width="19.7109375" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" customWidth="1"/>
+    <col min="20" max="20" width="18.5703125" customWidth="1"/>
+    <col min="22" max="22" width="25" customWidth="1"/>
+    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
         <v>4</v>
       </c>
@@ -854,449 +863,464 @@
         <v>4</v>
       </c>
       <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" t="s">
         <v>105</v>
       </c>
-      <c r="N2" t="s">
+      <c r="S2" t="s">
         <v>76</v>
       </c>
-      <c r="O2" t="s">
+      <c r="T2" t="s">
         <v>67</v>
       </c>
-      <c r="P2" t="s">
+      <c r="U2" t="s">
         <v>44</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="V2" t="s">
         <v>39</v>
       </c>
-      <c r="R2" t="s">
+      <c r="W2" t="s">
         <v>23</v>
       </c>
-      <c r="S2" t="s">
+      <c r="X2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="H3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="I3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="J3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="K3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
+      <c r="L3" t="s">
         <v>36</v>
       </c>
-      <c r="H3" t="s">
+      <c r="M3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" t="s">
+      <c r="N3" t="s">
         <v>75</v>
       </c>
-      <c r="J3" t="s">
+      <c r="O3" t="s">
         <v>91</v>
       </c>
-      <c r="K3" t="s">
+      <c r="P3" t="s">
         <v>17</v>
       </c>
-      <c r="L3" t="s">
+      <c r="Q3" t="s">
         <v>3</v>
       </c>
-      <c r="M3" t="s">
+      <c r="R3" t="s">
         <v>106</v>
       </c>
-      <c r="N3" t="s">
+      <c r="S3" t="s">
         <v>77</v>
       </c>
-      <c r="O3" t="s">
+      <c r="T3" t="s">
         <v>68</v>
       </c>
-      <c r="P3" t="s">
+      <c r="U3" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="V3" t="s">
         <v>40</v>
       </c>
-      <c r="R3" t="s">
+      <c r="W3" t="s">
         <v>24</v>
       </c>
-      <c r="S3" t="s">
+      <c r="X3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="H4" t="s">
         <v>30</v>
       </c>
-      <c r="D4" t="s">
+      <c r="I4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="J4" t="s">
         <v>38</v>
       </c>
-      <c r="F4" t="s">
+      <c r="K4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
+      <c r="L4" t="s">
         <v>37</v>
       </c>
-      <c r="H4" t="s">
+      <c r="M4" t="s">
         <v>43</v>
       </c>
-      <c r="I4" t="s">
+      <c r="N4" t="s">
         <v>88</v>
       </c>
-      <c r="J4" t="s">
+      <c r="O4" t="s">
         <v>3</v>
       </c>
-      <c r="K4" t="s">
+      <c r="P4" t="s">
         <v>95</v>
       </c>
-      <c r="L4" t="s">
+      <c r="Q4" t="s">
         <v>1</v>
       </c>
-      <c r="M4" t="s">
+      <c r="R4" t="s">
         <v>107</v>
       </c>
-      <c r="N4" t="s">
+      <c r="S4" t="s">
         <v>78</v>
       </c>
-      <c r="O4" t="s">
+      <c r="T4" t="s">
         <v>69</v>
       </c>
-      <c r="S4" t="s">
+      <c r="X4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="G5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="H5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="I5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
+      <c r="J5" t="s">
         <v>56</v>
       </c>
-      <c r="F5" t="s">
+      <c r="K5" t="s">
         <v>27</v>
       </c>
-      <c r="H5" t="s">
+      <c r="M5" t="s">
         <v>73</v>
       </c>
-      <c r="I5" t="s">
+      <c r="N5" t="s">
         <v>89</v>
       </c>
-      <c r="J5" t="s">
+      <c r="O5" t="s">
         <v>1</v>
       </c>
-      <c r="K5" t="s">
+      <c r="P5" t="s">
         <v>1</v>
       </c>
-      <c r="L5" t="s">
+      <c r="Q5" t="s">
         <v>57</v>
       </c>
-      <c r="N5" t="s">
+      <c r="S5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="G6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
+      <c r="H6" t="s">
         <v>32</v>
       </c>
-      <c r="E6" t="s">
+      <c r="J6" t="s">
         <v>26</v>
       </c>
-      <c r="F6" t="s">
+      <c r="K6" t="s">
         <v>28</v>
       </c>
-      <c r="H6" t="s">
+      <c r="M6" t="s">
         <v>74</v>
       </c>
-      <c r="I6" t="s">
+      <c r="N6" t="s">
         <v>104</v>
       </c>
-      <c r="J6" t="s">
+      <c r="O6" t="s">
         <v>103</v>
       </c>
-      <c r="K6" t="s">
+      <c r="P6" t="s">
         <v>3</v>
       </c>
-      <c r="L6" t="s">
+      <c r="Q6" t="s">
         <v>55</v>
       </c>
-      <c r="N6" t="s">
+      <c r="S6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="G7" t="s">
         <v>50</v>
       </c>
-      <c r="C7" t="s">
+      <c r="H7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
+      <c r="J7" t="s">
         <v>65</v>
       </c>
-      <c r="F7" t="s">
+      <c r="K7" t="s">
         <v>31</v>
       </c>
-      <c r="I7" t="s">
+      <c r="N7" t="s">
         <v>122</v>
       </c>
-      <c r="J7" t="s">
+      <c r="O7" t="s">
         <v>102</v>
       </c>
-      <c r="K7" t="s">
+      <c r="P7" t="s">
         <v>36</v>
       </c>
-      <c r="L7" t="s">
+      <c r="Q7" t="s">
         <v>50</v>
       </c>
-      <c r="N7" t="s">
+      <c r="S7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="G8" t="s">
         <v>122</v>
       </c>
-      <c r="E8" t="s">
+      <c r="J8" t="s">
         <v>71</v>
       </c>
-      <c r="I8" t="s">
+      <c r="N8" t="s">
         <v>124</v>
       </c>
-      <c r="J8" t="s">
+      <c r="O8" t="s">
         <v>101</v>
       </c>
-      <c r="K8" t="s">
+      <c r="P8" t="s">
         <v>114</v>
       </c>
-      <c r="L8" t="s">
+      <c r="Q8" t="s">
         <v>58</v>
       </c>
-      <c r="N8" t="s">
+      <c r="S8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
+      <c r="G9" t="s">
         <v>124</v>
       </c>
-      <c r="J9" t="s">
+      <c r="O9" t="s">
         <v>100</v>
       </c>
-      <c r="K9" t="s">
+      <c r="P9" t="s">
         <v>96</v>
       </c>
-      <c r="L9" t="s">
+      <c r="Q9" t="s">
         <v>59</v>
       </c>
-      <c r="N9" t="s">
+      <c r="S9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
         <v>33</v>
       </c>
-      <c r="K10" t="s">
+      <c r="P10" t="s">
         <v>97</v>
       </c>
-      <c r="N10" t="s">
+      <c r="S10" t="s">
         <v>84</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="V10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
         <v>34</v>
       </c>
-      <c r="J11" t="s">
+      <c r="O11" t="s">
         <v>92</v>
       </c>
-      <c r="K11" t="s">
+      <c r="P11" t="s">
         <v>98</v>
       </c>
-      <c r="N11" t="s">
+      <c r="S11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
         <v>35</v>
       </c>
-      <c r="J12" t="s">
+      <c r="O12" t="s">
         <v>93</v>
       </c>
-      <c r="K12" t="s">
+      <c r="P12" t="s">
         <v>99</v>
       </c>
-      <c r="N12" t="s">
+      <c r="S12" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
         <v>46</v>
       </c>
-      <c r="C13" t="s">
+      <c r="H13" t="s">
         <v>72</v>
       </c>
-      <c r="K13" t="s">
+      <c r="P13" t="s">
         <v>118</v>
       </c>
-      <c r="N13" t="s">
+      <c r="S13" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
         <v>47</v>
       </c>
-      <c r="K14" t="s">
+      <c r="P14" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
         <v>48</v>
       </c>
-      <c r="K15" t="s">
+      <c r="P15" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
         <v>49</v>
       </c>
-      <c r="K16" t="s">
+      <c r="P16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K17" t="s">
+    <row r="17" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F18" t="s">
+    <row r="18" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
         <v>66</v>
       </c>
-      <c r="K18" t="s">
+      <c r="P18" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="19" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="6:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I22" t="s">
+    <row r="22" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E23" t="s">
+    <row r="23" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
         <v>70</v>
       </c>
-      <c r="I23" t="s">
+      <c r="N23" t="s">
         <v>109</v>
       </c>
-      <c r="L23" t="s">
+      <c r="Q23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I24" t="s">
+    <row r="24" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
         <v>110</v>
       </c>
-      <c r="K24" t="s">
+      <c r="P24" t="s">
         <v>117</v>
       </c>
-      <c r="L24" t="s">
+      <c r="Q24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I25" t="s">
+    <row r="25" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="N25" t="s">
         <v>111</v>
       </c>
-      <c r="L25" t="s">
+      <c r="Q25" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I26" t="s">
+    <row r="26" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="N26" t="s">
         <v>112</v>
       </c>
-      <c r="L26" t="s">
+      <c r="Q26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I27" t="s">
+    <row r="27" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="N27" t="s">
         <v>113</v>
       </c>
-      <c r="L27" t="s">
+      <c r="Q27" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B28">
+    <row r="28" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="G28">
         <v>1010001</v>
       </c>
-      <c r="I28" t="s">
+      <c r="N28" t="s">
         <v>123</v>
       </c>
-      <c r="L28" t="s">
+      <c r="Q28" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>